<commit_message>
Add test data for nan case
</commit_message>
<xml_diff>
--- a/tests/data/testSet.xlsx
+++ b/tests/data/testSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e1719a4fc7bdcc1/datos_aldo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23CFBD68-3A83-47C6-A60D-1527CD9F6AC5}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9D5541F3-BAC8-4B23-970F-B48E77996D9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BDF2ABE-C379-42E0-84CD-A644370E78C0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="18">
   <si>
     <t>TestSet1</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>lat = -2.25; lon = -77.45</t>
+  </si>
+  <si>
+    <t>TestSet9</t>
+  </si>
+  <si>
+    <t>TestSet10</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>lat = -9.95; lon = -80.45</t>
   </si>
 </sst>
 </file>
@@ -449,14 +461,14 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="21" width="9.140625" style="3"/>
+    <col min="2" max="11" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="9.140625" style="3"/>
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -485,6 +497,12 @@
       <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -517,6 +535,12 @@
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -549,6 +573,12 @@
       <c r="I3" s="3">
         <v>10</v>
       </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>10</v>
+      </c>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -581,6 +611,12 @@
       <c r="I4" s="3">
         <v>72.863754</v>
       </c>
+      <c r="J4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -613,6 +649,12 @@
       <c r="I5" s="3">
         <v>109.169281</v>
       </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
@@ -645,6 +687,12 @@
       <c r="I6" s="3">
         <v>78.134345999999994</v>
       </c>
+      <c r="J6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -677,6 +725,12 @@
       <c r="I7" s="3">
         <v>92.655388000000002</v>
       </c>
+      <c r="J7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -709,6 +763,12 @@
       <c r="I8" s="3">
         <v>102.545433</v>
       </c>
+      <c r="J8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -741,6 +801,12 @@
       <c r="I9" s="3">
         <v>119.120811</v>
       </c>
+      <c r="J9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -773,6 +839,12 @@
       <c r="I10" s="3">
         <v>82.187201999999999</v>
       </c>
+      <c r="J10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -805,6 +877,12 @@
       <c r="I11" s="3">
         <v>80.651138000000003</v>
       </c>
+      <c r="J11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -837,6 +915,12 @@
       <c r="I12" s="3">
         <v>251.345169</v>
       </c>
+      <c r="J12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -869,6 +953,12 @@
       <c r="I13" s="3">
         <v>106.985237</v>
       </c>
+      <c r="J13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -901,6 +991,12 @@
       <c r="I14" s="3">
         <v>48.404162999999997</v>
       </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -933,6 +1029,12 @@
       <c r="I15" s="3">
         <v>46.834915000000002</v>
       </c>
+      <c r="J15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -965,6 +1067,12 @@
       <c r="I16" s="3">
         <v>114.40166499999999</v>
       </c>
+      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -997,6 +1105,12 @@
       <c r="I17" s="3">
         <v>90.154822999999993</v>
       </c>
+      <c r="J17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1029,6 +1143,12 @@
       <c r="I18" s="3">
         <v>88.333939000000001</v>
       </c>
+      <c r="J18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -1061,6 +1181,12 @@
       <c r="I19" s="3">
         <v>137.26542699999999</v>
       </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -1093,6 +1219,12 @@
       <c r="I20" s="3">
         <v>96.217681999999996</v>
       </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -1125,6 +1257,12 @@
       <c r="I21" s="3">
         <v>175.81632999999999</v>
       </c>
+      <c r="J21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -1157,6 +1295,12 @@
       <c r="I22" s="3">
         <v>90.339668000000003</v>
       </c>
+      <c r="J22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -1189,6 +1333,12 @@
       <c r="I23" s="3">
         <v>56.076873999999997</v>
       </c>
+      <c r="J23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -1221,6 +1371,12 @@
       <c r="I24" s="3">
         <v>91.339859000000004</v>
       </c>
+      <c r="J24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -1253,6 +1409,12 @@
       <c r="I25" s="3">
         <v>128.82577499999999</v>
       </c>
+      <c r="J25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -1285,6 +1447,12 @@
       <c r="I26" s="3">
         <v>100.077461</v>
       </c>
+      <c r="J26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -1317,6 +1485,12 @@
       <c r="I27" s="3">
         <v>130.94544999999999</v>
       </c>
+      <c r="J27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -1349,6 +1523,12 @@
       <c r="I28" s="3">
         <v>100.002945</v>
       </c>
+      <c r="J28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -1381,6 +1561,12 @@
       <c r="I29" s="3">
         <v>97.807372999999998</v>
       </c>
+      <c r="J29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
@@ -1413,6 +1599,12 @@
       <c r="I30" s="3">
         <v>103.89923899999999</v>
       </c>
+      <c r="J30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -1445,6 +1637,12 @@
       <c r="I31" s="3">
         <v>104.597977</v>
       </c>
+      <c r="J31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -1477,6 +1675,12 @@
       <c r="I32" s="3">
         <v>68.260475</v>
       </c>
+      <c r="J32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
@@ -1509,6 +1713,12 @@
       <c r="I33" s="3">
         <v>92.294158999999993</v>
       </c>
+      <c r="J33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -1541,6 +1751,12 @@
       <c r="I34" s="3">
         <v>99.177834000000004</v>
       </c>
+      <c r="J34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
@@ -1573,6 +1789,12 @@
       <c r="I35" s="3">
         <v>114.084137</v>
       </c>
+      <c r="J35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
@@ -1605,6 +1827,12 @@
       <c r="I36" s="3">
         <v>112.101181</v>
       </c>
+      <c r="J36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
@@ -1637,6 +1865,12 @@
       <c r="I37" s="3">
         <v>99.053650000000005</v>
       </c>
+      <c r="J37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -1669,6 +1903,12 @@
       <c r="I38" s="3">
         <v>78.526473999999993</v>
       </c>
+      <c r="J38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
@@ -1700,6 +1940,12 @@
       </c>
       <c r="I39" s="3">
         <v>87.148582000000005</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>

</xml_diff>

<commit_message>
Add another test case to increase coverage
</commit_message>
<xml_diff>
--- a/tests/data/testSet.xlsx
+++ b/tests/data/testSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e1719a4fc7bdcc1/datos_aldo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9D5541F3-BAC8-4B23-970F-B48E77996D9E}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{02F6227D-26F2-480A-B59F-9C8E6EC4C9FA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BDF2ABE-C379-42E0-84CD-A644370E78C0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
   <si>
     <t>TestSet1</t>
   </si>
@@ -89,12 +89,18 @@
   <si>
     <t>lat = -9.95; lon = -80.45</t>
   </si>
+  <si>
+    <t>lat = -3.45; lon = -73.75</t>
+  </si>
+  <si>
+    <t>TestSet11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +114,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,14 +473,14 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="21" width="9.140625" style="3"/>
+    <col min="2" max="12" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="9.140625" style="3"/>
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -503,6 +515,9 @@
       <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -541,6 +556,9 @@
       <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -579,6 +597,9 @@
       <c r="K3" s="3">
         <v>10</v>
       </c>
+      <c r="L3" s="3">
+        <v>2</v>
+      </c>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -617,6 +638,9 @@
       <c r="K4" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L4" s="3">
+        <v>193.874481</v>
+      </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -655,6 +679,9 @@
       <c r="K5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L5" s="3">
+        <v>316.611694</v>
+      </c>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
@@ -693,6 +720,9 @@
       <c r="K6" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L6" s="3">
+        <v>171.66679400000001</v>
+      </c>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -731,6 +761,9 @@
       <c r="K7" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L7" s="3">
+        <v>201.692352</v>
+      </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -769,6 +802,9 @@
       <c r="K8" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L8" s="3">
+        <v>144.96560700000001</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -807,6 +843,9 @@
       <c r="K9" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L9" s="3">
+        <v>158.298508</v>
+      </c>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -845,6 +884,9 @@
       <c r="K10" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L10" s="3">
+        <v>190.596924</v>
+      </c>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -883,6 +925,9 @@
       <c r="K11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L11" s="3">
+        <v>184.66799900000001</v>
+      </c>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -921,6 +966,9 @@
       <c r="K12" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L12" s="3">
+        <v>248.916641</v>
+      </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -959,6 +1007,9 @@
       <c r="K13" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L13" s="3">
+        <v>190.74238600000001</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -997,6 +1048,9 @@
       <c r="K14" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L14" s="3">
+        <v>173.46260100000001</v>
+      </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -1035,6 +1089,9 @@
       <c r="K15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L15" s="3">
+        <v>186.179642</v>
+      </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -1073,6 +1130,9 @@
       <c r="K16" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L16" s="3">
+        <v>179.836884</v>
+      </c>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -1111,6 +1171,9 @@
       <c r="K17" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L17" s="3">
+        <v>229.54093900000001</v>
+      </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1149,6 +1212,9 @@
       <c r="K18" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L18" s="3">
+        <v>199.62600699999999</v>
+      </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -1187,6 +1253,9 @@
       <c r="K19" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L19" s="3">
+        <v>205.67482000000001</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -1225,6 +1294,9 @@
       <c r="K20" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L20" s="3">
+        <v>313.57409699999999</v>
+      </c>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -1263,6 +1335,9 @@
       <c r="K21" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L21" s="3">
+        <v>266.92361499999998</v>
+      </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -1301,6 +1376,9 @@
       <c r="K22" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L22" s="3">
+        <v>240.54885899999999</v>
+      </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -1339,6 +1417,9 @@
       <c r="K23" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L23" s="3">
+        <v>214.20491000000001</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -1377,6 +1458,9 @@
       <c r="K24" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L24" s="3">
+        <v>239.843613</v>
+      </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -1415,6 +1499,9 @@
       <c r="K25" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L25" s="3">
+        <v>220.60766599999999</v>
+      </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -1453,6 +1540,9 @@
       <c r="K26" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L26" s="3">
+        <v>182.49731399999999</v>
+      </c>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -1491,6 +1581,9 @@
       <c r="K27" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L27" s="3">
+        <v>184.14544699999999</v>
+      </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -1529,6 +1622,9 @@
       <c r="K28" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L28" s="3">
+        <v>214.069748</v>
+      </c>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -1567,6 +1663,9 @@
       <c r="K29" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L29" s="3">
+        <v>180.03396599999999</v>
+      </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
@@ -1605,6 +1704,9 @@
       <c r="K30" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L30" s="3">
+        <v>103.624382</v>
+      </c>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -1643,6 +1745,9 @@
       <c r="K31" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L31" s="3">
+        <v>244.55023199999999</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -1681,6 +1786,9 @@
       <c r="K32" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L32" s="3">
+        <v>319.81076000000002</v>
+      </c>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
@@ -1719,6 +1827,9 @@
       <c r="K33" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L33" s="3">
+        <v>151.56395000000001</v>
+      </c>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -1757,6 +1868,9 @@
       <c r="K34" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L34" s="3">
+        <v>172.67053200000001</v>
+      </c>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
@@ -1795,6 +1909,9 @@
       <c r="K35" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L35" s="3">
+        <v>290.80294800000001</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
@@ -1833,6 +1950,9 @@
       <c r="K36" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L36" s="3">
+        <v>301.14794899999998</v>
+      </c>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
@@ -1871,6 +1991,9 @@
       <c r="K37" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L37" s="3">
+        <v>161.75573700000001</v>
+      </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -1909,6 +2032,9 @@
       <c r="K38" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L38" s="3">
+        <v>239.582596</v>
+      </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
@@ -1947,11 +2073,15 @@
       <c r="K39" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="L39" s="3">
+        <v>330.86465500000003</v>
+      </c>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add test case for pvalue of 0.1
</commit_message>
<xml_diff>
--- a/tests/data/testSet.xlsx
+++ b/tests/data/testSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e1719a4fc7bdcc1/datos_aldo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{02F6227D-26F2-480A-B59F-9C8E6EC4C9FA}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{54BE55EC-096D-4804-A45D-5357F67DD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E04A2FEC-B5C5-4767-A51C-61C144E790B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BDF2ABE-C379-42E0-84CD-A644370E78C0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="22">
   <si>
     <t>TestSet1</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>TestSet11</t>
+  </si>
+  <si>
+    <t>TestSet12</t>
+  </si>
+  <si>
+    <t>lat = -3.95; lon = -76.45</t>
   </si>
 </sst>
 </file>
@@ -473,14 +479,14 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M4" sqref="M4:M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="9.140625" style="3"/>
+    <col min="2" max="13" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="9.140625" style="3"/>
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -518,6 +524,9 @@
       <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -559,6 +568,9 @@
       <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -600,6 +612,9 @@
       <c r="L3" s="3">
         <v>2</v>
       </c>
+      <c r="M3" s="3">
+        <v>3</v>
+      </c>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -641,6 +656,9 @@
       <c r="L4" s="3">
         <v>193.874481</v>
       </c>
+      <c r="M4" s="3">
+        <v>268.91250600000001</v>
+      </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -682,6 +700,9 @@
       <c r="L5" s="3">
         <v>316.611694</v>
       </c>
+      <c r="M5" s="3">
+        <v>161.081909</v>
+      </c>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
@@ -723,6 +744,9 @@
       <c r="L6" s="3">
         <v>171.66679400000001</v>
       </c>
+      <c r="M6" s="3">
+        <v>357.21743800000002</v>
+      </c>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -764,6 +788,9 @@
       <c r="L7" s="3">
         <v>201.692352</v>
       </c>
+      <c r="M7" s="3">
+        <v>249.054214</v>
+      </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -805,6 +832,9 @@
       <c r="L8" s="3">
         <v>144.96560700000001</v>
       </c>
+      <c r="M8" s="3">
+        <v>229.525238</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -846,6 +876,9 @@
       <c r="L9" s="3">
         <v>158.298508</v>
       </c>
+      <c r="M9" s="3">
+        <v>244.09295700000001</v>
+      </c>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -887,6 +920,9 @@
       <c r="L10" s="3">
         <v>190.596924</v>
       </c>
+      <c r="M10" s="3">
+        <v>195.20970199999999</v>
+      </c>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -928,6 +964,9 @@
       <c r="L11" s="3">
         <v>184.66799900000001</v>
       </c>
+      <c r="M11" s="3">
+        <v>151.659897</v>
+      </c>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -969,6 +1008,9 @@
       <c r="L12" s="3">
         <v>248.916641</v>
       </c>
+      <c r="M12" s="3">
+        <v>302.43261699999999</v>
+      </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -1010,6 +1052,9 @@
       <c r="L13" s="3">
         <v>190.74238600000001</v>
       </c>
+      <c r="M13" s="3">
+        <v>137.18383800000001</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -1051,6 +1096,9 @@
       <c r="L14" s="3">
         <v>173.46260100000001</v>
       </c>
+      <c r="M14" s="3">
+        <v>280.87658699999997</v>
+      </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -1092,6 +1140,9 @@
       <c r="L15" s="3">
         <v>186.179642</v>
       </c>
+      <c r="M15" s="3">
+        <v>238.31366</v>
+      </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -1133,6 +1184,9 @@
       <c r="L16" s="3">
         <v>179.836884</v>
       </c>
+      <c r="M16" s="3">
+        <v>393.60635400000001</v>
+      </c>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -1174,6 +1228,9 @@
       <c r="L17" s="3">
         <v>229.54093900000001</v>
       </c>
+      <c r="M17" s="3">
+        <v>233.70457500000001</v>
+      </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1215,6 +1272,9 @@
       <c r="L18" s="3">
         <v>199.62600699999999</v>
       </c>
+      <c r="M18" s="3">
+        <v>291.595123</v>
+      </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -1256,6 +1316,9 @@
       <c r="L19" s="3">
         <v>205.67482000000001</v>
       </c>
+      <c r="M19" s="3">
+        <v>232.639938</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -1297,6 +1360,9 @@
       <c r="L20" s="3">
         <v>313.57409699999999</v>
       </c>
+      <c r="M20" s="3">
+        <v>286.830444</v>
+      </c>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -1338,6 +1404,9 @@
       <c r="L21" s="3">
         <v>266.92361499999998</v>
       </c>
+      <c r="M21" s="3">
+        <v>287.28903200000002</v>
+      </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -1379,6 +1448,9 @@
       <c r="L22" s="3">
         <v>240.54885899999999</v>
       </c>
+      <c r="M22" s="3">
+        <v>246.88320899999999</v>
+      </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -1420,6 +1492,9 @@
       <c r="L23" s="3">
         <v>214.20491000000001</v>
       </c>
+      <c r="M23" s="3">
+        <v>260.78558299999997</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -1461,6 +1536,9 @@
       <c r="L24" s="3">
         <v>239.843613</v>
       </c>
+      <c r="M24" s="3">
+        <v>295.37292500000001</v>
+      </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -1502,6 +1580,9 @@
       <c r="L25" s="3">
         <v>220.60766599999999</v>
       </c>
+      <c r="M25" s="3">
+        <v>313.68679800000001</v>
+      </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -1543,6 +1624,9 @@
       <c r="L26" s="3">
         <v>182.49731399999999</v>
       </c>
+      <c r="M26" s="3">
+        <v>165.817093</v>
+      </c>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -1584,6 +1668,9 @@
       <c r="L27" s="3">
         <v>184.14544699999999</v>
       </c>
+      <c r="M27" s="3">
+        <v>153.329407</v>
+      </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -1625,6 +1712,9 @@
       <c r="L28" s="3">
         <v>214.069748</v>
       </c>
+      <c r="M28" s="3">
+        <v>200.539917</v>
+      </c>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -1666,6 +1756,9 @@
       <c r="L29" s="3">
         <v>180.03396599999999</v>
       </c>
+      <c r="M29" s="3">
+        <v>298.24316399999998</v>
+      </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
@@ -1707,6 +1800,9 @@
       <c r="L30" s="3">
         <v>103.624382</v>
       </c>
+      <c r="M30" s="3">
+        <v>190.00320400000001</v>
+      </c>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -1748,6 +1844,9 @@
       <c r="L31" s="3">
         <v>244.55023199999999</v>
       </c>
+      <c r="M31" s="3">
+        <v>190.03788800000001</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -1789,6 +1888,9 @@
       <c r="L32" s="3">
         <v>319.81076000000002</v>
       </c>
+      <c r="M32" s="3">
+        <v>256.82815599999998</v>
+      </c>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
@@ -1830,6 +1932,9 @@
       <c r="L33" s="3">
         <v>151.56395000000001</v>
       </c>
+      <c r="M33" s="3">
+        <v>242.30514500000001</v>
+      </c>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -1871,6 +1976,9 @@
       <c r="L34" s="3">
         <v>172.67053200000001</v>
       </c>
+      <c r="M34" s="3">
+        <v>218.93104600000001</v>
+      </c>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
@@ -1912,6 +2020,9 @@
       <c r="L35" s="3">
         <v>290.80294800000001</v>
       </c>
+      <c r="M35" s="3">
+        <v>221.66009500000001</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
@@ -1953,6 +2064,9 @@
       <c r="L36" s="3">
         <v>301.14794899999998</v>
       </c>
+      <c r="M36" s="3">
+        <v>264.14392099999998</v>
+      </c>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
@@ -1994,6 +2108,9 @@
       <c r="L37" s="3">
         <v>161.75573700000001</v>
       </c>
+      <c r="M37" s="3">
+        <v>196.86462399999999</v>
+      </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -2035,6 +2152,9 @@
       <c r="L38" s="3">
         <v>239.582596</v>
       </c>
+      <c r="M38" s="3">
+        <v>333.99807700000002</v>
+      </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
@@ -2075,6 +2195,9 @@
       </c>
       <c r="L39" s="3">
         <v>330.86465500000003</v>
+      </c>
+      <c r="M39" s="3">
+        <v>219.888443</v>
       </c>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>

</xml_diff>